<commit_message>
add import master line
</commit_message>
<xml_diff>
--- a/public/assets/example/contoh-import-master-plan.xlsx
+++ b/public/assets/example/contoh-import-master-plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20400" windowHeight="7620"/>
+    <workbookView windowWidth="19545" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -731,7 +731,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1259,7 +1259,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>